<commit_message>
Updated Tank Building Instructions
</commit_message>
<xml_diff>
--- a/Models/Tank/Tank_BOM.xlsx
+++ b/Models/Tank/Tank_BOM.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="57">
   <si>
     <t>Brick</t>
   </si>
@@ -38,10 +38,19 @@
     <t>194 - Medium Stone Grey</t>
   </si>
   <si>
-    <t>4297187</t>
-  </si>
-  <si>
-    <t>Cable 208mm</t>
+    <t>4502834</t>
+  </si>
+  <si>
+    <t>CATERPILLAR TRACK</t>
+  </si>
+  <si>
+    <t>26 - Black</t>
+  </si>
+  <si>
+    <t>6024583</t>
+  </si>
+  <si>
+    <t>CABLE 350 MM</t>
   </si>
   <si>
     <t>40 - Transparent, 26 - Black</t>
@@ -65,6 +74,15 @@
     <t>208 - Light Stone Grey</t>
   </si>
   <si>
+    <t>4168114</t>
+  </si>
+  <si>
+    <t>TECHNIC ANG. BEAM 4X2 90 DEG</t>
+  </si>
+  <si>
+    <t>23 - Bright Blue</t>
+  </si>
+  <si>
     <t>4297202</t>
   </si>
   <si>
@@ -101,15 +119,21 @@
     <t>DOUBLE ANGULAR BEAM 3X7 45°</t>
   </si>
   <si>
+    <t>4239601</t>
+  </si>
+  <si>
+    <t>1/2 BUSH</t>
+  </si>
+  <si>
+    <t>24 - Bright Yellow</t>
+  </si>
+  <si>
     <t>4121715</t>
   </si>
   <si>
     <t>CONNECTOR PEG W. FRICTION</t>
   </si>
   <si>
-    <t>26 - Black</t>
-  </si>
-  <si>
     <t>4211622</t>
   </si>
   <si>
@@ -122,25 +146,31 @@
     <t>CONN.BUSH W.FRIC./CROSSALE</t>
   </si>
   <si>
-    <t>23 - Bright Blue</t>
-  </si>
-  <si>
-    <t>370526</t>
-  </si>
-  <si>
-    <t>CROSS AXLE 4M</t>
-  </si>
-  <si>
-    <t>655826</t>
+    <t>4514553</t>
   </si>
   <si>
     <t>CONNECTOR PEG W. FRICTION 3M</t>
   </si>
   <si>
-    <t>4211865</t>
-  </si>
-  <si>
-    <t>2M FRIC. SNAP W/CROSS HOLE</t>
+    <t>6031821</t>
+  </si>
+  <si>
+    <t>CROSSAXLE 3M WITH KNOB</t>
+  </si>
+  <si>
+    <t>138 - Sand Yellow</t>
+  </si>
+  <si>
+    <t>4211639</t>
+  </si>
+  <si>
+    <t>CROSS AXLE 5M</t>
+  </si>
+  <si>
+    <t>370626</t>
+  </si>
+  <si>
+    <t>CROSS AXLE 6M</t>
   </si>
   <si>
     <t>4296059</t>
@@ -215,7 +245,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="4297187 Screenshot" descr="4297187"/>
+        <xdr:cNvPr id="3" name="4502834 Screenshot" descr="4502834"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -259,7 +289,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="4297008 Screenshot" descr="4297008"/>
+        <xdr:cNvPr id="4" name="6024583 Screenshot" descr="6024583"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -303,7 +333,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="4297199 Screenshot" descr="4297199"/>
+        <xdr:cNvPr id="5" name="4297008 Screenshot" descr="4297008"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -347,7 +377,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="4297202 Screenshot" descr="4297202"/>
+        <xdr:cNvPr id="6" name="4297199 Screenshot" descr="4297199"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -391,7 +421,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="4522937 Screenshot" descr="4522937"/>
+        <xdr:cNvPr id="7" name="4168114 Screenshot" descr="4168114"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -435,7 +465,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="4297203 Screenshot" descr="4297203"/>
+        <xdr:cNvPr id="8" name="4297202 Screenshot" descr="4297202"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -479,7 +509,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="4297197 Screenshot" descr="4297197"/>
+        <xdr:cNvPr id="9" name="4522937 Screenshot" descr="4522937"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -523,7 +553,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="4210753 Screenshot" descr="4210753"/>
+        <xdr:cNvPr id="10" name="4297203 Screenshot" descr="4297203"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -567,7 +597,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="4210668 Screenshot" descr="4210668"/>
+        <xdr:cNvPr id="11" name="4297197 Screenshot" descr="4297197"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -611,7 +641,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="4121715 Screenshot" descr="4121715"/>
+        <xdr:cNvPr id="12" name="4210753 Screenshot" descr="4210753"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -655,7 +685,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="4211622 Screenshot" descr="4211622"/>
+        <xdr:cNvPr id="13" name="4210668 Screenshot" descr="4210668"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -699,7 +729,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="4206482 Screenshot" descr="4206482"/>
+        <xdr:cNvPr id="14" name="4239601 Screenshot" descr="4239601"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -743,7 +773,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="370526 Screenshot" descr="370526"/>
+        <xdr:cNvPr id="15" name="4121715 Screenshot" descr="4121715"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -787,7 +817,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="655826 Screenshot" descr="655826"/>
+        <xdr:cNvPr id="16" name="4211622 Screenshot" descr="4211622"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -831,7 +861,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="4211865 Screenshot" descr="4211865"/>
+        <xdr:cNvPr id="17" name="4206482 Screenshot" descr="4206482"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -875,7 +905,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="4296059 Screenshot" descr="4296059"/>
+        <xdr:cNvPr id="18" name="4514553 Screenshot" descr="4514553"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -895,6 +925,182 @@
       <xdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:off x="3448050" y="14449425"/>
+          <a:ext cx="813600" cy="813600"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>755650</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>812800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="6031821 Screenshot" descr="6031821"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image18">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3448050" y="15287625"/>
+          <a:ext cx="813600" cy="813600"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>755650</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>812800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="4211639 Screenshot" descr="4211639"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image19">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3448050" y="16125825"/>
+          <a:ext cx="813600" cy="813600"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>755650</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>812800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="370626 Screenshot" descr="370626"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image20">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3448050" y="16964025"/>
+          <a:ext cx="813600" cy="813600"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>755650</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>812800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="4296059 Screenshot" descr="4296059"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" r:embed="image21">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3448050" y="17802225"/>
           <a:ext cx="813600" cy="813600"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
@@ -909,7 +1115,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -966,7 +1172,7 @@
         <v>10</v>
       </c>
       <c r="D3">
-        <v>55804</v>
+        <v>53992</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -983,7 +1189,7 @@
         <v>13</v>
       </c>
       <c r="D4">
-        <v>53787</v>
+        <v>11146</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
@@ -1000,7 +1206,7 @@
         <v>16</v>
       </c>
       <c r="D5">
-        <v>32524</v>
+        <v>53787</v>
       </c>
       <c r="E5" t="s">
         <v>17</v>
@@ -1017,10 +1223,10 @@
         <v>19</v>
       </c>
       <c r="D6">
-        <v>40490</v>
+        <v>32524</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F6">
         <v>2</v>
@@ -1028,33 +1234,33 @@
     </row>
     <row r="7" spans="1:6" ht="66" customHeight="1">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D7">
-        <v>41239</v>
+        <v>32140</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="66" customHeight="1">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D8">
-        <v>41239</v>
+        <v>40490</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F8">
         <v>2</v>
@@ -1062,50 +1268,50 @@
     </row>
     <row r="9" spans="1:6" ht="66" customHeight="1">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D9">
-        <v>32278</v>
+        <v>41239</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="66" customHeight="1">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
         <v>27</v>
       </c>
       <c r="D10">
-        <v>32526</v>
+        <v>41239</v>
       </c>
       <c r="E10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F10">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="66" customHeight="1">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D11">
-        <v>32009</v>
+        <v>32278</v>
       </c>
       <c r="E11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F11">
         <v>2</v>
@@ -1113,33 +1319,33 @@
     </row>
     <row r="12" spans="1:6" ht="66" customHeight="1">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D12">
-        <v>2780</v>
+        <v>32526</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F12">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="66" customHeight="1">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D13">
-        <v>6590</v>
+        <v>32009</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="F13">
         <v>4</v>
@@ -1147,50 +1353,50 @@
     </row>
     <row r="14" spans="1:6" ht="66" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D14">
-        <v>43093</v>
+        <v>32123</v>
       </c>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F14">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="66" customHeight="1">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D15">
-        <v>3705</v>
+        <v>2780</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="F15">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="66" customHeight="1">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D16">
-        <v>6558</v>
+        <v>6590</v>
       </c>
       <c r="E16" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="F16">
         <v>2</v>
@@ -1198,16 +1404,16 @@
     </row>
     <row r="17" spans="1:6" ht="66" customHeight="1">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D17">
-        <v>32054</v>
+        <v>43093</v>
       </c>
       <c r="E17" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F17">
         <v>4</v>
@@ -1215,27 +1421,95 @@
     </row>
     <row r="18" spans="1:6" ht="66" customHeight="1">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D18">
+        <v>6558</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="66" customHeight="1">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19">
+        <v>6587</v>
+      </c>
+      <c r="E19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="66" customHeight="1">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20">
+        <v>32073</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="66" customHeight="1">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21">
+        <v>3706</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="66" customHeight="1">
+      <c r="A22" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22">
         <v>55615</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E22" t="s">
         <v>8</v>
       </c>
-      <c r="F18">
+      <c r="F22">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
-      <c r="A19" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19">
-        <f>SUM(F2:F18)</f>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23">
+        <f>SUM(F2:F22)</f>
       </c>
     </row>
   </sheetData>

</xml_diff>